<commit_message>
finish Appendices 13th April
</commit_message>
<xml_diff>
--- a/stats/bryum/month_PAR_stats_X1.xlsx
+++ b/stats/bryum/month_PAR_stats_X1.xlsx
@@ -1,40 +1,59 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s2096910_ed_ac_uk/Documents/dissertation/dissertation/dissertation/stats/bryum/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_60C6943CD88FE829B3731BA9862D48F8E3F4F45F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEFF61CB-93B0-6A4A-9FEE-8F6D6B66311D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
-    <t xml:space="preserve">Year</t>
+    <t>Year</t>
   </si>
   <si>
-    <t xml:space="preserve">Month</t>
+    <t>Month</t>
   </si>
   <si>
-    <t xml:space="preserve">mean_PAR</t>
+    <t>mean_PAR</t>
   </si>
   <si>
-    <t xml:space="preserve">max_PAR</t>
+    <t>max_PAR</t>
   </si>
   <si>
-    <t xml:space="preserve">min_PAR</t>
+    <t>min_PAR</t>
+  </si>
+  <si>
+    <t>Bryum_X1</t>
+  </si>
+  <si>
+    <t>Bryum_X2</t>
+  </si>
+  <si>
+    <t>Bryum_X4</t>
+  </si>
+  <si>
+    <t>Austroplaca_X3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -63,13 +82,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -351,304 +383,796 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:N18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="15" width="10.83203125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+      <c r="F2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>2019</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B3">
         <v>11</v>
       </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>9.1666666666666397E-2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>6</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1.3513888888888901</v>
+      </c>
+      <c r="M3" s="2">
+        <v>18</v>
+      </c>
+      <c r="N3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>2019</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B4">
         <v>12</v>
       </c>
-      <c r="C3" t="n">
-        <v>164.873655913978</v>
-      </c>
-      <c r="D3" t="n">
+      <c r="C4" s="2">
+        <v>164.87365591397801</v>
+      </c>
+      <c r="D4" s="2">
         <v>1170</v>
       </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>286.25806451612601</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2116</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>160.46236559139899</v>
+      </c>
+      <c r="J4" s="2">
+        <v>605</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>212.30107526881699</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1091</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>2020</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B5">
         <v>1</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C5" s="2">
         <v>417.825503355705</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D5" s="2">
         <v>1249</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E5" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
+      <c r="F5" s="2">
+        <v>428.51409395973099</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2015</v>
+      </c>
+      <c r="H5" s="2">
+        <v>27</v>
+      </c>
+      <c r="I5" s="2">
+        <v>229.327516778524</v>
+      </c>
+      <c r="J5" s="2">
+        <v>881</v>
+      </c>
+      <c r="K5" s="2">
+        <v>6</v>
+      </c>
+      <c r="L5" s="2">
+        <v>183.25369127516799</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1084</v>
+      </c>
+      <c r="N5" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>2020</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B6">
         <v>2</v>
       </c>
-      <c r="C5" t="n">
-        <v>102.26724137931</v>
-      </c>
-      <c r="D5" t="n">
+      <c r="C6" s="2">
+        <v>102.26724137930999</v>
+      </c>
+      <c r="D6" s="2">
         <v>863</v>
       </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>135.05603448275801</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1508</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>69.899425287356394</v>
+      </c>
+      <c r="J6" s="2">
+        <v>710</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>46.4410919540232</v>
+      </c>
+      <c r="M6" s="2">
+        <v>598</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>2020</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B7">
         <v>11</v>
       </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1.38888888888889E-3</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>5.5555555555554699E-2</v>
+      </c>
+      <c r="M7" s="2">
+        <v>4</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>2020</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B8">
         <v>12</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C8" s="2">
         <v>148.189516129033</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D8" s="2">
         <v>868</v>
       </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>285.00403225806502</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2036</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>131.35349462365701</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1114</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <v>181.793010752687</v>
+      </c>
+      <c r="M8" s="2">
+        <v>1143</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>2021</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B9">
         <v>1</v>
       </c>
-      <c r="C8" t="n">
-        <v>349.369623655914</v>
-      </c>
-      <c r="D8" t="n">
+      <c r="C9" s="2">
+        <v>349.36962365591398</v>
+      </c>
+      <c r="D9" s="2">
         <v>915</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E9" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
+      <c r="F9" s="2">
+        <v>313.55510752688099</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1968</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2</v>
+      </c>
+      <c r="I9" s="2">
+        <v>259.43010752688201</v>
+      </c>
+      <c r="J9" s="2">
+        <v>977</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>188.64247311828001</v>
+      </c>
+      <c r="M9" s="2">
+        <v>1253</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>2021</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B10">
         <v>2</v>
       </c>
-      <c r="C9" t="n">
-        <v>33.9360119047622</v>
-      </c>
-      <c r="D9" t="n">
+      <c r="C10" s="2">
+        <v>33.936011904762204</v>
+      </c>
+      <c r="D10" s="2">
         <v>760</v>
       </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>18.2842261904762</v>
+      </c>
+      <c r="G10" s="2">
+        <v>486</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>22.988095238095099</v>
+      </c>
+      <c r="J10" s="2">
+        <v>873</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>13.504464285714199</v>
+      </c>
+      <c r="M10" s="2">
+        <v>498</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>2021</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B11">
         <v>11</v>
       </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1.38888888888889E-3</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1.38888888888889E-3</v>
+      </c>
+      <c r="M11" s="2">
+        <v>1</v>
+      </c>
+      <c r="N11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>2021</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B12">
         <v>12</v>
       </c>
-      <c r="C11" t="n">
-        <v>242.400537634408</v>
-      </c>
-      <c r="D11" t="n">
+      <c r="C12" s="2">
+        <v>242.40053763440801</v>
+      </c>
+      <c r="D12" s="2">
         <v>1015</v>
       </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>238.51478494623601</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1718</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>114.297043010753</v>
+      </c>
+      <c r="J12" s="2">
+        <v>585</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>151.98521505376399</v>
+      </c>
+      <c r="M12" s="2">
+        <v>1012</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>2022</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B13">
         <v>1</v>
       </c>
-      <c r="C12" t="n">
-        <v>449.961021505376</v>
-      </c>
-      <c r="D12" t="n">
+      <c r="C13" s="2">
+        <v>449.96102150537598</v>
+      </c>
+      <c r="D13" s="2">
         <v>1257</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E13" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
+      <c r="F13" s="2">
+        <v>387.01075268817101</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1625</v>
+      </c>
+      <c r="H13" s="2">
+        <v>33</v>
+      </c>
+      <c r="I13" s="2">
+        <v>264.25</v>
+      </c>
+      <c r="J13" s="2">
+        <v>946</v>
+      </c>
+      <c r="K13" s="2">
+        <v>21</v>
+      </c>
+      <c r="L13" s="2">
+        <v>207.24865591397801</v>
+      </c>
+      <c r="M13" s="2">
+        <v>1360</v>
+      </c>
+      <c r="N13" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>2022</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B14">
         <v>2</v>
       </c>
-      <c r="C13" t="n">
-        <v>136.813988095239</v>
-      </c>
-      <c r="D13" t="n">
+      <c r="C14" s="2">
+        <v>136.81398809523901</v>
+      </c>
+      <c r="D14" s="2">
         <v>815</v>
       </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>112.224702380951</v>
+      </c>
+      <c r="G14" s="2">
+        <v>652</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <v>79.912202380951896</v>
+      </c>
+      <c r="J14" s="2">
+        <v>579</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
+        <v>54.775297619047599</v>
+      </c>
+      <c r="M14" s="2">
+        <v>662</v>
+      </c>
+      <c r="N14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>2022</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B15">
         <v>11</v>
       </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1.2055555555555599</v>
+      </c>
+      <c r="G15" s="2">
+        <v>34</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0.23749999999999899</v>
+      </c>
+      <c r="M15" s="2">
+        <v>16</v>
+      </c>
+      <c r="N15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>2022</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B16">
         <v>12</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C16" s="2">
         <v>212.008064516129</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D16" s="2">
         <v>1201</v>
       </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>399.96236559139902</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1542</v>
+      </c>
+      <c r="H16" s="2">
+        <v>7</v>
+      </c>
+      <c r="I16" s="2">
+        <v>201.84274193548299</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1042</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2">
+        <v>155.21102150537601</v>
+      </c>
+      <c r="M16" s="2">
+        <v>837</v>
+      </c>
+      <c r="N16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17">
         <v>2023</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B17">
         <v>1</v>
       </c>
-      <c r="C16" t="n">
-        <v>348.416666666667</v>
-      </c>
-      <c r="D16" t="n">
+      <c r="C17" s="2">
+        <v>348.41666666666703</v>
+      </c>
+      <c r="D17" s="2">
         <v>1152</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E17" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
+      <c r="F17" s="2">
+        <v>391.96370967741899</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1701</v>
+      </c>
+      <c r="H17" s="2">
+        <v>6</v>
+      </c>
+      <c r="I17" s="2">
+        <v>340.73790322580601</v>
+      </c>
+      <c r="J17" s="2">
+        <v>994</v>
+      </c>
+      <c r="K17" s="2">
+        <v>2</v>
+      </c>
+      <c r="L17" s="2">
+        <v>181.287634408602</v>
+      </c>
+      <c r="M17" s="2">
+        <v>960</v>
+      </c>
+      <c r="N17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>2023</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B18">
         <v>2</v>
       </c>
-      <c r="C17" t="n">
-        <v>174.619970193741</v>
-      </c>
-      <c r="D17" t="n">
+      <c r="C18" s="2">
+        <v>174.61997019374101</v>
+      </c>
+      <c r="D18" s="2">
         <v>682</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>170.04321907600601</v>
+      </c>
+      <c r="G18" s="2">
+        <v>716</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>165.461997019374</v>
+      </c>
+      <c r="J18" s="2">
+        <v>865</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2">
+        <v>91.976154992548501</v>
+      </c>
+      <c r="M18" s="2">
+        <v>575</v>
+      </c>
+      <c r="N18" s="2">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:N1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>